<commit_message>
Updated the Ninja skills doc. Evrything got kind of normalysed and ready to contignous in the Elementalist skills doc.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/Done/3_Ninja/Documentation/NinjaSkills.xlsx
+++ b/GameDesign/Class/Done/3_Ninja/Documentation/NinjaSkills.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="81">
   <si>
     <t>[[MP: 0 ]]</t>
   </si>
@@ -80,9 +80,6 @@
     <t>Effect name: ''Geta''.</t>
   </si>
   <si>
-    <t>When walking over glyph or trap, dosn't activate them.</t>
-  </si>
-  <si>
     <t>[[AP: 3 ]]</t>
   </si>
   <si>
@@ -188,18 +185,12 @@
     <t>*The poison effect is there if the spell was used whit ''Cyanide''. Even if the player don't have ''Cyanide'' the other turn, the poison is applyed.                                                                                                          *If the player used this spell whitout ''Cyanide'', the spell will not apply poison, even if the player as the ''Cyanide'' effect.</t>
   </si>
   <si>
-    <t>Glyph (3 turns)</t>
-  </si>
-  <si>
     <t>[[Damage:  25 earth ]]</t>
   </si>
   <si>
     <t>If under ''Cyanide'' effect: [[Poison +1 lvl on target ]] (2 turns)</t>
   </si>
   <si>
-    <t>The damage are triggered at the start of a target turn on the area and for each of its moving into a makibishi cell.</t>
-  </si>
-  <si>
     <t>[[Area of effect: - Circle of 4 cell radius ]] (60% rate per cell in area)</t>
   </si>
   <si>
@@ -218,9 +209,6 @@
     <t>[[Area of effect: - 4 adjacent cell of the targeted cell]]</t>
   </si>
   <si>
-    <t>Can only use the skill on a cell adjacent of an big obstacle between the player and the targeted cell.</t>
-  </si>
-  <si>
     <t>[[Damage:  10 air ]] (Affect only enemies)</t>
   </si>
   <si>
@@ -254,9 +242,6 @@
     <t>[[Max effect accumulation: 3 ]]</t>
   </si>
   <si>
-    <t>When take distance damage, decrase ''Tatami'' by 1 lvl and reduct the damage to 0.</t>
-  </si>
-  <si>
     <t>[[Tatami +3lvl ]] (1 turns)</t>
   </si>
   <si>
@@ -266,28 +251,31 @@
     <t>Protect the target from glyph, trap and field effect.</t>
   </si>
   <si>
-    <t>Increases the target's MP. The MP bonus is less effective on allies than on the caster himself.</t>
-  </si>
-  <si>
-    <t>Inflicts Earth-type damage. If under Cyanide effect, also give poisons that inflicts Dark-type damage.</t>
-  </si>
-  <si>
-    <t>Inflicts Air-type damage. If under Cyanide effect, also give poisons that inflicts Dark-type damage.</t>
-  </si>
-  <si>
-    <t>Inflicts Air-type damage. If under Cyanide effect, also give poisons that inflicts Dark-type damage.                                                 Reduces the target power and resistances.</t>
-  </si>
-  <si>
-    <t>Inflicts Earth-type damage. If used under Cyanide effect, also give poisons that inflicts Dark-type damage.                                        Every cells in the area has a chance to lay a makibishi.                 The affected cell dealt damage when an entity start his turn on it or when crossed.</t>
-  </si>
-  <si>
     <t>Teleports onto the targeted cell.                                                 Inflicts Air-type damage on enemies between the initial caster position and its final position.                                                          Can only be used on cells adjacent and on the other side of a big obstacle.</t>
   </si>
   <si>
-    <t>Reduces the target's skills AP cost for the current turn but increases  the target's skills AP cost the following turn.</t>
-  </si>
-  <si>
     <t>Reduces to 0 the target taken damage from distance for few hits.</t>
+  </si>
+  <si>
+    <t>Increases the target's MP.                                                                The MP bonus is less effective on allies than on the caster.</t>
+  </si>
+  <si>
+    <t>Inflicts Earth-type damage and when under Cyanide effect, also give poisons that inflicts Dark-type damage.</t>
+  </si>
+  <si>
+    <t>Inflicts Air-type damage and when under Cyanide effect, also give poisons that inflicts Dark-type damage.</t>
+  </si>
+  <si>
+    <t>Inflicts Air-type damage and when under Cyanide effect, also give poisons that inflicts Dark-type damage.                                                 Reduces the target power and resistances.</t>
+  </si>
+  <si>
+    <t>Inflicts Earth-type damage and when used under Cyanide effect, also give poisons that inflicts Dark-type damage.                                        Every cells in the area has a chance to lay a makibishi.                 The affected cell dealt damage when an entity start his turn on it or when crossed.</t>
+  </si>
+  <si>
+    <t>Active Glyph (3 turns)</t>
+  </si>
+  <si>
+    <t>Reduces the target's skills AP cost for the current turn but increases  the target's skills AP cost the next turn.</t>
   </si>
 </sst>
 </file>
@@ -327,7 +315,7 @@
       <family val="5"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -349,12 +337,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -404,7 +386,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -425,22 +407,19 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -789,8 +768,8 @@
     </row>
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="15" t="s">
-        <v>75</v>
+      <c r="C5" s="12" t="s">
+        <v>70</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -918,10 +897,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D26"/>
+  <dimension ref="B2:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,7 +920,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -953,7 +932,7 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -965,21 +944,21 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -1003,14 +982,14 @@
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1034,7 +1013,7 @@
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -1061,24 +1040,17 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
       <c r="C24" s="9" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
-      <c r="C25" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="6"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1087,346 +1059,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D26"/>
-  <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="2.85546875" customWidth="1"/>
-    <col min="3" max="3" width="85.7109375" customWidth="1"/>
-    <col min="4" max="6" width="2.85546875" customWidth="1"/>
-    <col min="7" max="7" width="78.5703125" customWidth="1"/>
-    <col min="8" max="8" width="2.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B7" s="1"/>
-      <c r="C7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B10" s="1"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B11" s="1"/>
-      <c r="C11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B12" s="1"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B14" s="1"/>
-      <c r="C14" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B18" s="1"/>
-      <c r="C18" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B22" s="1"/>
-      <c r="C22" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B24" s="1"/>
-      <c r="C24" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B25" s="1"/>
-      <c r="C25" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D26"/>
-  <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="2.85546875" customWidth="1"/>
-    <col min="3" max="3" width="85.7109375" customWidth="1"/>
-    <col min="4" max="6" width="2.85546875" customWidth="1"/>
-    <col min="7" max="7" width="78.5703125" customWidth="1"/>
-    <col min="8" max="8" width="2.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
-      <c r="B5" s="1"/>
-      <c r="C5" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B7" s="1"/>
-      <c r="C7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B10" s="1"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B11" s="1"/>
-      <c r="C11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B12" s="1"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B14" s="1"/>
-      <c r="C14" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B18" s="1"/>
-      <c r="C18" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B23" s="1"/>
-      <c r="C23" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B25" s="1"/>
-      <c r="C25" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D25"/>
   <sheetViews>
@@ -1451,7 +1083,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1460,10 +1092,10 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="15" t="s">
-        <v>78</v>
+      <c r="C5" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1475,14 +1107,347 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>28</v>
+        <v>16</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B9" s="1"/>
+      <c r="C9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B10" s="1"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B11" s="1"/>
+      <c r="C11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B12" s="1"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B13" s="1"/>
+      <c r="C13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B14" s="1"/>
+      <c r="C14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B15" s="1"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B16" s="1"/>
+      <c r="C16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B18" s="1"/>
+      <c r="C18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B22" s="1"/>
+      <c r="C22" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B24" s="1"/>
+      <c r="C24" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D26"/>
+  <sheetViews>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="2.85546875" customWidth="1"/>
+    <col min="3" max="3" width="85.7109375" customWidth="1"/>
+    <col min="4" max="6" width="2.85546875" customWidth="1"/>
+    <col min="7" max="7" width="78.5703125" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="1"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+      <c r="C5" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B8" s="1"/>
+      <c r="C8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B9" s="1"/>
+      <c r="C9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B10" s="1"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B11" s="1"/>
+      <c r="C11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B12" s="1"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B13" s="1"/>
+      <c r="C13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B14" s="1"/>
+      <c r="C14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B15" s="1"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B16" s="1"/>
+      <c r="C16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B18" s="1"/>
+      <c r="C18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B19" s="1"/>
+      <c r="C19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B23" s="1"/>
+      <c r="C23" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B25" s="1"/>
+      <c r="C25" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D25"/>
+  <sheetViews>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="2.85546875" customWidth="1"/>
+    <col min="3" max="3" width="85.7109375" customWidth="1"/>
+    <col min="4" max="6" width="2.85546875" customWidth="1"/>
+    <col min="7" max="7" width="78.5703125" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="1"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
+      <c r="B5" s="1"/>
+      <c r="C5" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B8" s="1"/>
+      <c r="C8" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1506,14 +1471,14 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -1529,22 +1494,22 @@
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
-      <c r="C17" s="3" t="s">
-        <v>63</v>
+      <c r="C17" s="14" t="s">
+        <v>59</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="3" t="s">
-        <v>39</v>
+      <c r="C18" s="14" t="s">
+        <v>38</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -1612,7 +1577,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1623,8 +1588,8 @@
     </row>
     <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="15" t="s">
-        <v>79</v>
+      <c r="C5" s="12" t="s">
+        <v>76</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1636,7 +1601,7 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" s="1"/>
     </row>
@@ -1650,7 +1615,7 @@
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -1662,21 +1627,21 @@
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -1688,14 +1653,14 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -1711,22 +1676,22 @@
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B21" s="1"/>
+      <c r="C21" s="14" t="s">
         <v>37</v>
-      </c>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B21" s="1"/>
-      <c r="C21" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -1774,7 +1739,7 @@
   <dimension ref="B2:D29"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1794,7 +1759,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1805,8 +1770,8 @@
     </row>
     <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="15" t="s">
-        <v>80</v>
+      <c r="C5" s="12" t="s">
+        <v>77</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1818,14 +1783,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1837,21 +1802,21 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -1863,14 +1828,14 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -1886,36 +1851,36 @@
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>43</v>
+      <c r="C19" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B21" s="1"/>
+      <c r="C21" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B21" s="1"/>
-      <c r="C21" s="10" t="s">
-        <v>46</v>
-      </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>38</v>
+      <c r="C22" s="14" t="s">
+        <v>37</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -1945,7 +1910,7 @@
     <row r="28" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B28" s="1"/>
       <c r="C28" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D28" s="1"/>
     </row>
@@ -1962,10 +1927,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D28"/>
+  <dimension ref="B2:D27"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1985,7 +1950,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1996,8 +1961,8 @@
     </row>
     <row r="5" spans="2:4" ht="97.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="15" t="s">
-        <v>81</v>
+      <c r="C5" s="12" t="s">
+        <v>78</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2009,14 +1974,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -2028,21 +1993,21 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -2054,7 +2019,7 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -2066,7 +2031,7 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -2078,21 +2043,21 @@
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="3" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="D20" s="1"/>
     </row>
@@ -2121,22 +2086,15 @@
     </row>
     <row r="26" spans="2:4" ht="98.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
-      <c r="C26" s="12" t="s">
-        <v>50</v>
+      <c r="C26" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="39" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
-      <c r="C27" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="6"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2149,7 +2107,7 @@
   <dimension ref="B2:D27"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2169,7 +2127,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2180,8 +2138,8 @@
     </row>
     <row r="5" spans="2:4" ht="97.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="15" t="s">
-        <v>82</v>
+      <c r="C5" s="12" t="s">
+        <v>72</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2193,21 +2151,21 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -2219,21 +2177,21 @@
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -2245,7 +2203,7 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -2257,7 +2215,7 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -2269,14 +2227,14 @@
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D20" s="1"/>
     </row>
@@ -2303,11 +2261,9 @@
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" ht="39" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
-      <c r="C26" s="13" t="s">
-        <v>61</v>
-      </c>
+      <c r="C26" s="11"/>
       <c r="D26" s="1"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
@@ -2346,7 +2302,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2357,8 +2313,8 @@
     </row>
     <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="15" t="s">
-        <v>83</v>
+      <c r="C5" s="12" t="s">
+        <v>80</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2377,14 +2333,14 @@
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -2408,7 +2364,7 @@
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -2439,14 +2395,14 @@
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -2476,14 +2432,14 @@
     <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
       <c r="C25" s="9" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
       <c r="C26" s="9" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D26" s="1"/>
     </row>

</xml_diff>